<commit_message>
fix bugs templates and download file
</commit_message>
<xml_diff>
--- a/src/assets/documents/Template-BaseResidencial-FallasRR.xlsx
+++ b/src/assets/documents/Template-BaseResidencial-FallasRR.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
   <si>
     <t>CUENTA</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>MATRIZ</t>
+  </si>
+  <si>
+    <t>INCIDENTE</t>
   </si>
 </sst>
 </file>
@@ -2428,8 +2431,8 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>